<commit_message>
fix(import): Mise à jour de l'import suite à l'ajout des numéros de téléphones etrangers
</commit_message>
<xml_diff>
--- a/packages/backend/src/_static/usagers-import-test/import_ok_1.xlsx
+++ b/packages/backend/src/_static/usagers-import-test/import_ok_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/_static/usagers-import-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7718FAA7-3E01-F540-9C1D-2F4A216C0EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE565F5D-43FA-9D47-8427-E3DC968E1E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-12800" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -511,63 +511,6 @@
     <t>06/05/2017</t>
   </si>
   <si>
-    <t>0101010101</t>
-  </si>
-  <si>
-    <t>0101010102</t>
-  </si>
-  <si>
-    <t>0101010103</t>
-  </si>
-  <si>
-    <t>0101010104</t>
-  </si>
-  <si>
-    <t>0101010105</t>
-  </si>
-  <si>
-    <t>0101010106</t>
-  </si>
-  <si>
-    <t>0101010107</t>
-  </si>
-  <si>
-    <t>0101010108</t>
-  </si>
-  <si>
-    <t>0101010109</t>
-  </si>
-  <si>
-    <t>0101010110</t>
-  </si>
-  <si>
-    <t>0101010111</t>
-  </si>
-  <si>
-    <t>0101010112</t>
-  </si>
-  <si>
-    <t>0101010113</t>
-  </si>
-  <si>
-    <t>0101010114</t>
-  </si>
-  <si>
-    <t>0101010115</t>
-  </si>
-  <si>
-    <t>0101010116</t>
-  </si>
-  <si>
-    <t>0101010117</t>
-  </si>
-  <si>
-    <t>0101010118</t>
-  </si>
-  <si>
-    <t>0101010119</t>
-  </si>
-  <si>
     <t>Sénégal</t>
   </si>
   <si>
@@ -578,6 +521,63 @@
   </si>
   <si>
     <t>Si lien commune</t>
+  </si>
+  <si>
+    <t>0601010101</t>
+  </si>
+  <si>
+    <t>0601010102</t>
+  </si>
+  <si>
+    <t>0601010103</t>
+  </si>
+  <si>
+    <t>0601010104</t>
+  </si>
+  <si>
+    <t>0601010105</t>
+  </si>
+  <si>
+    <t>0601010106</t>
+  </si>
+  <si>
+    <t>0601010107</t>
+  </si>
+  <si>
+    <t>0601010108</t>
+  </si>
+  <si>
+    <t>0601010109</t>
+  </si>
+  <si>
+    <t>0601010110</t>
+  </si>
+  <si>
+    <t>0601010111</t>
+  </si>
+  <si>
+    <t>0601010112</t>
+  </si>
+  <si>
+    <t>0601010113</t>
+  </si>
+  <si>
+    <t>0601010114</t>
+  </si>
+  <si>
+    <t>0601010115</t>
+  </si>
+  <si>
+    <t>0601010116</t>
+  </si>
+  <si>
+    <t>0601010117</t>
+  </si>
+  <si>
+    <t>0601010118</t>
+  </si>
+  <si>
+    <t>0601010119</t>
   </si>
 </sst>
 </file>
@@ -970,7 +970,7 @@
   <dimension ref="A1:AX20"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+      <selection activeCell="H2" sqref="H2:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1064,7 +1064,7 @@
         <v>22</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>23</v>
@@ -1156,7 +1156,7 @@
         <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E2" t="s">
         <v>87</v>
@@ -1165,10 +1165,10 @@
         <v>88</v>
       </c>
       <c r="G2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="I2" t="s">
         <v>50</v>
@@ -1230,7 +1230,7 @@
         <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E3" t="s">
         <v>87</v>
@@ -1239,10 +1239,10 @@
         <v>93</v>
       </c>
       <c r="G3" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="I3" t="s">
         <v>50</v>
@@ -1301,7 +1301,7 @@
         <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E4" t="s">
         <v>87</v>
@@ -1310,10 +1310,10 @@
         <v>95</v>
       </c>
       <c r="G4" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="I4" t="s">
         <v>50</v>
@@ -1372,7 +1372,7 @@
         <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E5" t="s">
         <v>87</v>
@@ -1381,10 +1381,10 @@
         <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="I5" t="s">
         <v>50</v>
@@ -1446,7 +1446,7 @@
         <v>87</v>
       </c>
       <c r="D6" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E6" t="s">
         <v>87</v>
@@ -1455,10 +1455,10 @@
         <v>103</v>
       </c>
       <c r="G6" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="I6" t="s">
         <v>50</v>
@@ -1520,7 +1520,7 @@
         <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E7" t="s">
         <v>87</v>
@@ -1529,10 +1529,10 @@
         <v>108</v>
       </c>
       <c r="G7" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="I7" t="s">
         <v>50</v>
@@ -1591,7 +1591,7 @@
         <v>87</v>
       </c>
       <c r="D8" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E8" t="s">
         <v>87</v>
@@ -1600,10 +1600,10 @@
         <v>113</v>
       </c>
       <c r="G8" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="I8" t="s">
         <v>50</v>
@@ -1662,7 +1662,7 @@
         <v>87</v>
       </c>
       <c r="D9" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E9" t="s">
         <v>87</v>
@@ -1671,10 +1671,10 @@
         <v>115</v>
       </c>
       <c r="G9" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I9" t="s">
         <v>50</v>
@@ -1733,7 +1733,7 @@
         <v>87</v>
       </c>
       <c r="D10" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E10" t="s">
         <v>87</v>
@@ -1742,10 +1742,10 @@
         <v>119</v>
       </c>
       <c r="G10" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="I10" t="s">
         <v>50</v>
@@ -1804,7 +1804,7 @@
         <v>87</v>
       </c>
       <c r="D11" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E11" t="s">
         <v>87</v>
@@ -1813,10 +1813,10 @@
         <v>123</v>
       </c>
       <c r="G11" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="I11" t="s">
         <v>50</v>
@@ -1864,10 +1864,10 @@
         <v>58</v>
       </c>
       <c r="AI11" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="AJ11" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="AK11" s="3">
         <v>37951</v>
@@ -1876,10 +1876,10 @@
         <v>126</v>
       </c>
       <c r="AM11" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="AN11" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="AO11" s="3">
         <v>3953</v>
@@ -1899,7 +1899,7 @@
         <v>87</v>
       </c>
       <c r="D12" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E12" t="s">
         <v>87</v>
@@ -1908,10 +1908,10 @@
         <v>127</v>
       </c>
       <c r="G12" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="I12" t="s">
         <v>50</v>
@@ -1970,7 +1970,7 @@
         <v>87</v>
       </c>
       <c r="D13" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E13" t="s">
         <v>87</v>
@@ -1979,10 +1979,10 @@
         <v>130</v>
       </c>
       <c r="G13" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="I13" t="s">
         <v>50</v>
@@ -2041,7 +2041,7 @@
         <v>87</v>
       </c>
       <c r="D14" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E14" t="s">
         <v>87</v>
@@ -2050,10 +2050,10 @@
         <v>133</v>
       </c>
       <c r="G14" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="I14" t="s">
         <v>50</v>
@@ -2101,10 +2101,10 @@
         <v>58</v>
       </c>
       <c r="AI14" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="AJ14" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="AK14" s="3">
         <v>4751</v>
@@ -2124,7 +2124,7 @@
         <v>87</v>
       </c>
       <c r="D15" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E15" t="s">
         <v>87</v>
@@ -2133,10 +2133,10 @@
         <v>138</v>
       </c>
       <c r="G15" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="I15" t="s">
         <v>50</v>
@@ -2195,7 +2195,7 @@
         <v>87</v>
       </c>
       <c r="D16" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E16" t="s">
         <v>87</v>
@@ -2204,10 +2204,10 @@
         <v>142</v>
       </c>
       <c r="G16" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="I16" t="s">
         <v>50</v>
@@ -2266,7 +2266,7 @@
         <v>87</v>
       </c>
       <c r="D17" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E17" t="s">
         <v>87</v>
@@ -2275,10 +2275,10 @@
         <v>74</v>
       </c>
       <c r="G17" t="s">
+        <v>155</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>170</v>
       </c>
       <c r="I17" t="s">
         <v>50</v>
@@ -2337,7 +2337,7 @@
         <v>87</v>
       </c>
       <c r="D18" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E18" t="s">
         <v>87</v>
@@ -2346,10 +2346,10 @@
         <v>147</v>
       </c>
       <c r="G18" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="I18" t="s">
         <v>50</v>
@@ -2408,7 +2408,7 @@
         <v>87</v>
       </c>
       <c r="D19" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E19" t="s">
         <v>87</v>
@@ -2417,10 +2417,10 @@
         <v>150</v>
       </c>
       <c r="G19" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="I19" t="s">
         <v>50</v>
@@ -2479,7 +2479,7 @@
         <v>87</v>
       </c>
       <c r="D20" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E20" t="s">
         <v>87</v>
@@ -2488,10 +2488,10 @@
         <v>84</v>
       </c>
       <c r="G20" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="I20" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
fix(import): add new features to import
</commit_message>
<xml_diff>
--- a/packages/backend/src/_static/usagers-import-test/import_ok_1.xlsx
+++ b/packages/backend/src/_static/usagers-import-test/import_ok_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/_static/usagers-import-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE565F5D-43FA-9D47-8427-E3DC968E1E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E9B733-29FC-4C4F-9BF2-14E38CD017A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-12800" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,14 +18,15 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$AX$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$AY$1</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="181">
   <si>
     <t>ID 
 (colonne à remplir uniquement en cas d'ID personnalisés)</t>
@@ -579,12 +580,21 @@
   <si>
     <t>0601010119</t>
   </si>
+  <si>
+    <t>Quelle est la situation professionelle de la personne ?</t>
+  </si>
+  <si>
+    <t>SALARIE</t>
+  </si>
+  <si>
+    <t>FRANCE_TRAVAIL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,16 +608,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12.5"/>
+      <color rgb="FF262626"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F3F3"/>
+        <bgColor rgb="FFF3F3F3"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -615,11 +650,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -629,6 +679,12 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,9 +703,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -687,9 +743,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -722,26 +778,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -774,26 +813,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -967,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX20"/>
+  <dimension ref="A1:AY20"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H20"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -985,15 +1007,15 @@
     <col min="14" max="14" width="17.33203125" customWidth="1"/>
     <col min="15" max="15" width="25.6640625" customWidth="1"/>
     <col min="18" max="18" width="6.33203125" customWidth="1"/>
-    <col min="30" max="30" width="23" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="217" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.5" style="3"/>
-    <col min="41" max="41" width="11.5" style="3"/>
-    <col min="45" max="45" width="11.5" style="3"/>
-    <col min="49" max="49" width="11.5" style="3"/>
+    <col min="31" max="31" width="23" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="217" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.5" style="3"/>
+    <col min="42" max="42" width="11.5" style="3"/>
+    <col min="46" max="46" width="11.5" style="3"/>
+    <col min="50" max="50" width="11.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:51" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1054,98 +1076,101 @@
       <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:51" ht="17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1200,26 +1225,29 @@
       <c r="T2" t="s">
         <v>54</v>
       </c>
-      <c r="U2" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="U2" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="V2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z2" t="s">
         <v>55</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>56</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>57</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>58</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:51" ht="17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1274,23 +1302,26 @@
       <c r="T3" t="s">
         <v>54</v>
       </c>
-      <c r="U3" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y3" t="s">
+      <c r="U3" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="V3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z3" t="s">
         <v>65</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>56</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>57</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:51" ht="17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>6</v>
       </c>
@@ -1345,23 +1376,26 @@
       <c r="T4" t="s">
         <v>54</v>
       </c>
-      <c r="U4" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y4" t="s">
+      <c r="U4" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="V4" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z4" t="s">
         <v>55</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>56</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>57</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>11</v>
       </c>
@@ -1416,26 +1450,26 @@
       <c r="T5" t="s">
         <v>54</v>
       </c>
-      <c r="U5" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y5" t="s">
+      <c r="V5" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z5" t="s">
         <v>55</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>56</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>57</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>58</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>21</v>
       </c>
@@ -1490,26 +1524,26 @@
       <c r="T6" t="s">
         <v>54</v>
       </c>
-      <c r="U6" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y6" t="s">
+      <c r="V6" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z6" t="s">
         <v>65</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>56</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>57</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>58</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>29</v>
       </c>
@@ -1564,23 +1598,23 @@
       <c r="T7" t="s">
         <v>54</v>
       </c>
-      <c r="U7" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y7" t="s">
+      <c r="V7" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z7" t="s">
         <v>60</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>56</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>57</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>43</v>
       </c>
@@ -1635,23 +1669,23 @@
       <c r="T8" t="s">
         <v>54</v>
       </c>
-      <c r="U8" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y8" t="s">
+      <c r="V8" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z8" t="s">
         <v>55</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>56</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AC8" t="s">
         <v>57</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AE8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>44</v>
       </c>
@@ -1706,23 +1740,23 @@
       <c r="T9" t="s">
         <v>54</v>
       </c>
-      <c r="U9" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y9" t="s">
+      <c r="V9" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z9" t="s">
         <v>55</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AA9" t="s">
         <v>56</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AC9" t="s">
         <v>57</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AE9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>47</v>
       </c>
@@ -1777,23 +1811,23 @@
       <c r="T10" t="s">
         <v>54</v>
       </c>
-      <c r="U10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y10" t="s">
+      <c r="V10" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z10" t="s">
         <v>55</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AA10" t="s">
         <v>56</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AC10" t="s">
         <v>57</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AE10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>48</v>
       </c>
@@ -1848,47 +1882,47 @@
       <c r="T11" t="s">
         <v>54</v>
       </c>
-      <c r="U11" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y11" t="s">
+      <c r="V11" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z11" t="s">
         <v>64</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AA11" t="s">
         <v>56</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AC11" t="s">
         <v>57</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AE11" t="s">
         <v>58</v>
-      </c>
-      <c r="AI11" t="s">
-        <v>157</v>
       </c>
       <c r="AJ11" t="s">
         <v>157</v>
       </c>
-      <c r="AK11" s="3">
+      <c r="AK11" t="s">
+        <v>157</v>
+      </c>
+      <c r="AL11" s="3">
         <v>37951</v>
       </c>
-      <c r="AL11" t="s">
+      <c r="AM11" t="s">
         <v>126</v>
-      </c>
-      <c r="AM11" t="s">
-        <v>157</v>
       </c>
       <c r="AN11" t="s">
         <v>157</v>
       </c>
-      <c r="AO11" s="3">
+      <c r="AO11" t="s">
+        <v>157</v>
+      </c>
+      <c r="AP11" s="3">
         <v>3953</v>
       </c>
-      <c r="AP11" t="s">
+      <c r="AQ11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>54</v>
       </c>
@@ -1943,23 +1977,23 @@
       <c r="T12" t="s">
         <v>54</v>
       </c>
-      <c r="U12" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y12" t="s">
+      <c r="V12" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z12" t="s">
         <v>55</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="AA12" t="s">
         <v>56</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AC12" t="s">
         <v>57</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AE12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>77</v>
       </c>
@@ -2014,23 +2048,23 @@
       <c r="T13" t="s">
         <v>54</v>
       </c>
-      <c r="U13" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y13" t="s">
+      <c r="V13" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z13" t="s">
         <v>65</v>
       </c>
-      <c r="Z13" t="s">
+      <c r="AA13" t="s">
         <v>56</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AC13" t="s">
         <v>57</v>
       </c>
-      <c r="AD13" t="s">
+      <c r="AE13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>104</v>
       </c>
@@ -2085,35 +2119,35 @@
       <c r="T14" t="s">
         <v>54</v>
       </c>
-      <c r="U14" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y14" t="s">
+      <c r="V14" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z14" t="s">
         <v>64</v>
       </c>
-      <c r="Z14" t="s">
+      <c r="AA14" t="s">
         <v>56</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AC14" t="s">
         <v>57</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AE14" t="s">
         <v>58</v>
-      </c>
-      <c r="AI14" t="s">
-        <v>157</v>
       </c>
       <c r="AJ14" t="s">
         <v>157</v>
       </c>
-      <c r="AK14" s="3">
+      <c r="AK14" t="s">
+        <v>157</v>
+      </c>
+      <c r="AL14" s="3">
         <v>4751</v>
       </c>
-      <c r="AL14" t="s">
+      <c r="AM14" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>107</v>
       </c>
@@ -2168,23 +2202,23 @@
       <c r="T15" t="s">
         <v>54</v>
       </c>
-      <c r="U15" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y15" t="s">
+      <c r="V15" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z15" t="s">
         <v>67</v>
       </c>
-      <c r="Z15" t="s">
+      <c r="AA15" t="s">
         <v>56</v>
       </c>
-      <c r="AB15" t="s">
+      <c r="AC15" t="s">
         <v>57</v>
       </c>
-      <c r="AD15" t="s">
+      <c r="AE15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>116</v>
       </c>
@@ -2239,23 +2273,23 @@
       <c r="T16" t="s">
         <v>54</v>
       </c>
-      <c r="U16" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y16" t="s">
+      <c r="V16" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z16" t="s">
         <v>55</v>
       </c>
-      <c r="Z16" t="s">
+      <c r="AA16" t="s">
         <v>56</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AC16" t="s">
         <v>57</v>
       </c>
-      <c r="AD16" t="s">
+      <c r="AE16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>119</v>
       </c>
@@ -2310,23 +2344,23 @@
       <c r="T17" t="s">
         <v>54</v>
       </c>
-      <c r="U17" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y17" t="s">
+      <c r="V17" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z17" t="s">
         <v>55</v>
       </c>
-      <c r="Z17" t="s">
+      <c r="AA17" t="s">
         <v>56</v>
       </c>
-      <c r="AB17" t="s">
+      <c r="AC17" t="s">
         <v>57</v>
       </c>
-      <c r="AD17" t="s">
+      <c r="AE17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>131</v>
       </c>
@@ -2381,23 +2415,23 @@
       <c r="T18" t="s">
         <v>54</v>
       </c>
-      <c r="U18" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y18" t="s">
+      <c r="V18" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z18" t="s">
         <v>55</v>
       </c>
-      <c r="Z18" t="s">
+      <c r="AA18" t="s">
         <v>56</v>
       </c>
-      <c r="AB18" t="s">
+      <c r="AC18" t="s">
         <v>57</v>
       </c>
-      <c r="AD18" t="s">
+      <c r="AE18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>136</v>
       </c>
@@ -2452,23 +2486,23 @@
       <c r="T19" t="s">
         <v>54</v>
       </c>
-      <c r="U19" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y19" t="s">
+      <c r="V19" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z19" t="s">
         <v>55</v>
       </c>
-      <c r="Z19" t="s">
+      <c r="AA19" t="s">
         <v>56</v>
       </c>
-      <c r="AB19" t="s">
+      <c r="AC19" t="s">
         <v>57</v>
       </c>
-      <c r="AD19" t="s">
+      <c r="AE19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>140</v>
       </c>
@@ -2523,19 +2557,19 @@
       <c r="T20" t="s">
         <v>54</v>
       </c>
-      <c r="U20" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y20" t="s">
+      <c r="V20" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z20" t="s">
         <v>55</v>
       </c>
-      <c r="Z20" t="s">
+      <c r="AA20" t="s">
         <v>56</v>
       </c>
-      <c r="AB20" t="s">
+      <c r="AC20" t="s">
         <v>57</v>
       </c>
-      <c r="AD20" t="s">
+      <c r="AE20" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(import): add details pro situation
</commit_message>
<xml_diff>
--- a/packages/backend/src/_static/usagers-import-test/import_ok_1.xlsx
+++ b/packages/backend/src/_static/usagers-import-test/import_ok_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/_static/usagers-import-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E9B733-29FC-4C4F-9BF2-14E38CD017A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66D6313-33F4-8D47-B43D-DBF5DD711C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-12800" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,15 +18,14 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$AY$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$AZ$1</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="182">
   <si>
     <t>ID 
 (colonne à remplir uniquement en cas d'ID personnalisés)</t>
@@ -588,6 +587,9 @@
   </si>
   <si>
     <t>FRANCE_TRAVAIL</t>
+  </si>
+  <si>
+    <t>Si autre situation pro</t>
   </si>
 </sst>
 </file>
@@ -669,7 +671,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -683,6 +685,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -989,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AY20"/>
+  <dimension ref="A1:AZ20"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1007,15 +1015,15 @@
     <col min="14" max="14" width="17.33203125" customWidth="1"/>
     <col min="15" max="15" width="25.6640625" customWidth="1"/>
     <col min="18" max="18" width="6.33203125" customWidth="1"/>
-    <col min="31" max="31" width="23" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="217" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.5" style="3"/>
-    <col min="42" max="42" width="11.5" style="3"/>
-    <col min="46" max="46" width="11.5" style="3"/>
-    <col min="50" max="50" width="11.5" style="3"/>
+    <col min="32" max="32" width="23" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="217" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.5" style="3"/>
+    <col min="43" max="43" width="11.5" style="3"/>
+    <col min="47" max="47" width="11.5" style="3"/>
+    <col min="51" max="51" width="11.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1079,98 +1087,101 @@
       <c r="U1" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:51" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:52" ht="17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1228,26 +1239,27 @@
       <c r="U2" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="V2" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="V2" s="8"/>
+      <c r="W2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA2" t="s">
         <v>55</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>56</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>57</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>58</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:51" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:52" ht="17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1305,23 +1317,24 @@
       <c r="U3" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="V3" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z3" t="s">
+      <c r="V3" s="8"/>
+      <c r="W3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA3" t="s">
         <v>65</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>56</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>57</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:51" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:52" ht="17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>6</v>
       </c>
@@ -1379,23 +1392,24 @@
       <c r="U4" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="V4" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z4" t="s">
+      <c r="V4" s="8"/>
+      <c r="W4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA4" t="s">
         <v>55</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>56</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>57</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>11</v>
       </c>
@@ -1450,26 +1464,26 @@
       <c r="T5" t="s">
         <v>54</v>
       </c>
-      <c r="V5" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z5" t="s">
+      <c r="W5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA5" t="s">
         <v>55</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>56</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>57</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>58</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AJ5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>21</v>
       </c>
@@ -1524,26 +1538,26 @@
       <c r="T6" t="s">
         <v>54</v>
       </c>
-      <c r="V6" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z6" t="s">
+      <c r="W6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA6" t="s">
         <v>65</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>56</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>57</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>58</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>29</v>
       </c>
@@ -1598,23 +1612,23 @@
       <c r="T7" t="s">
         <v>54</v>
       </c>
-      <c r="V7" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z7" t="s">
+      <c r="W7" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA7" t="s">
         <v>60</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>56</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>57</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AF7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>43</v>
       </c>
@@ -1669,23 +1683,23 @@
       <c r="T8" t="s">
         <v>54</v>
       </c>
-      <c r="V8" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z8" t="s">
+      <c r="W8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA8" t="s">
         <v>55</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>56</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>57</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AF8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>44</v>
       </c>
@@ -1740,23 +1754,23 @@
       <c r="T9" t="s">
         <v>54</v>
       </c>
-      <c r="V9" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z9" t="s">
+      <c r="W9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA9" t="s">
         <v>55</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AB9" t="s">
         <v>56</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AD9" t="s">
         <v>57</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AF9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>47</v>
       </c>
@@ -1811,23 +1825,23 @@
       <c r="T10" t="s">
         <v>54</v>
       </c>
-      <c r="V10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z10" t="s">
+      <c r="W10" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA10" t="s">
         <v>55</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AB10" t="s">
         <v>56</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AD10" t="s">
         <v>57</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AF10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>48</v>
       </c>
@@ -1882,47 +1896,47 @@
       <c r="T11" t="s">
         <v>54</v>
       </c>
-      <c r="V11" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z11" t="s">
+      <c r="W11" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA11" t="s">
         <v>64</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AB11" t="s">
         <v>56</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AD11" t="s">
         <v>57</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AF11" t="s">
         <v>58</v>
-      </c>
-      <c r="AJ11" t="s">
-        <v>157</v>
       </c>
       <c r="AK11" t="s">
         <v>157</v>
       </c>
-      <c r="AL11" s="3">
+      <c r="AL11" t="s">
+        <v>157</v>
+      </c>
+      <c r="AM11" s="3">
         <v>37951</v>
       </c>
-      <c r="AM11" t="s">
+      <c r="AN11" t="s">
         <v>126</v>
-      </c>
-      <c r="AN11" t="s">
-        <v>157</v>
       </c>
       <c r="AO11" t="s">
         <v>157</v>
       </c>
-      <c r="AP11" s="3">
+      <c r="AP11" t="s">
+        <v>157</v>
+      </c>
+      <c r="AQ11" s="3">
         <v>3953</v>
       </c>
-      <c r="AQ11" t="s">
+      <c r="AR11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>54</v>
       </c>
@@ -1977,23 +1991,23 @@
       <c r="T12" t="s">
         <v>54</v>
       </c>
-      <c r="V12" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z12" t="s">
+      <c r="W12" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA12" t="s">
         <v>55</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AB12" t="s">
         <v>56</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AD12" t="s">
         <v>57</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AF12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>77</v>
       </c>
@@ -2048,23 +2062,23 @@
       <c r="T13" t="s">
         <v>54</v>
       </c>
-      <c r="V13" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z13" t="s">
+      <c r="W13" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA13" t="s">
         <v>65</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AB13" t="s">
         <v>56</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AD13" t="s">
         <v>57</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AF13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>104</v>
       </c>
@@ -2119,35 +2133,35 @@
       <c r="T14" t="s">
         <v>54</v>
       </c>
-      <c r="V14" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z14" t="s">
+      <c r="W14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA14" t="s">
         <v>64</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AB14" t="s">
         <v>56</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AD14" t="s">
         <v>57</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AF14" t="s">
         <v>58</v>
-      </c>
-      <c r="AJ14" t="s">
-        <v>157</v>
       </c>
       <c r="AK14" t="s">
         <v>157</v>
       </c>
-      <c r="AL14" s="3">
+      <c r="AL14" t="s">
+        <v>157</v>
+      </c>
+      <c r="AM14" s="3">
         <v>4751</v>
       </c>
-      <c r="AM14" t="s">
+      <c r="AN14" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>107</v>
       </c>
@@ -2202,23 +2216,23 @@
       <c r="T15" t="s">
         <v>54</v>
       </c>
-      <c r="V15" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z15" t="s">
+      <c r="W15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA15" t="s">
         <v>67</v>
       </c>
-      <c r="AA15" t="s">
+      <c r="AB15" t="s">
         <v>56</v>
       </c>
-      <c r="AC15" t="s">
+      <c r="AD15" t="s">
         <v>57</v>
       </c>
-      <c r="AE15" t="s">
+      <c r="AF15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>116</v>
       </c>
@@ -2273,23 +2287,23 @@
       <c r="T16" t="s">
         <v>54</v>
       </c>
-      <c r="V16" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z16" t="s">
+      <c r="W16" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA16" t="s">
         <v>55</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="AB16" t="s">
         <v>56</v>
       </c>
-      <c r="AC16" t="s">
+      <c r="AD16" t="s">
         <v>57</v>
       </c>
-      <c r="AE16" t="s">
+      <c r="AF16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>119</v>
       </c>
@@ -2344,23 +2358,23 @@
       <c r="T17" t="s">
         <v>54</v>
       </c>
-      <c r="V17" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z17" t="s">
+      <c r="W17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA17" t="s">
         <v>55</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="AB17" t="s">
         <v>56</v>
       </c>
-      <c r="AC17" t="s">
+      <c r="AD17" t="s">
         <v>57</v>
       </c>
-      <c r="AE17" t="s">
+      <c r="AF17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>131</v>
       </c>
@@ -2415,23 +2429,23 @@
       <c r="T18" t="s">
         <v>54</v>
       </c>
-      <c r="V18" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z18" t="s">
+      <c r="W18" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA18" t="s">
         <v>55</v>
       </c>
-      <c r="AA18" t="s">
+      <c r="AB18" t="s">
         <v>56</v>
       </c>
-      <c r="AC18" t="s">
+      <c r="AD18" t="s">
         <v>57</v>
       </c>
-      <c r="AE18" t="s">
+      <c r="AF18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>136</v>
       </c>
@@ -2486,23 +2500,23 @@
       <c r="T19" t="s">
         <v>54</v>
       </c>
-      <c r="V19" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z19" t="s">
+      <c r="W19" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA19" t="s">
         <v>55</v>
       </c>
-      <c r="AA19" t="s">
+      <c r="AB19" t="s">
         <v>56</v>
       </c>
-      <c r="AC19" t="s">
+      <c r="AD19" t="s">
         <v>57</v>
       </c>
-      <c r="AE19" t="s">
+      <c r="AF19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>140</v>
       </c>
@@ -2557,19 +2571,19 @@
       <c r="T20" t="s">
         <v>54</v>
       </c>
-      <c r="V20" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z20" t="s">
+      <c r="W20" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA20" t="s">
         <v>55</v>
       </c>
-      <c r="AA20" t="s">
+      <c r="AB20" t="s">
         <v>56</v>
       </c>
-      <c r="AC20" t="s">
+      <c r="AD20" t="s">
         <v>57</v>
       </c>
-      <c r="AE20" t="s">
+      <c r="AF20" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>